<commit_message>
Added tutorial no. 4 showing the use of the ODYM data format.
</commit_message>
<xml_diff>
--- a/ODYM_Classifications_Master_V10.xlsx
+++ b/ODYM_Classifications_Master_V10.xlsx
@@ -6553,10 +6553,10 @@
   <dimension ref="A1:AV1311"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="K18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="K38" sqref="K38"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7210,10 +7210,6 @@
       <c r="A8" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="7" t="str">
-        <f>Time_Discrete_Years!A8</f>
-        <v>Last modified by</v>
-      </c>
       <c r="C8" s="7" t="str">
         <f>Time_Discrete_Years!B8</f>
         <v>Stefan Pauliuk</v>
@@ -7291,10 +7287,6 @@
       <c r="A9" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="7" t="str">
-        <f>Time_Discrete_Years!A9</f>
-        <v>Reference</v>
-      </c>
       <c r="C9" s="7" t="str">
         <f>Time_Discrete_Years!B9</f>
         <v>None</v>
@@ -7303,7 +7295,10 @@
         <f>Chemical_Elements!B9</f>
         <v>0</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="7" t="str">
+        <f>SSP_Scenarios!B9</f>
+        <v xml:space="preserve">https://tntcat.iiasa.ac.at/SspDb/dsd?Action=htmlpage&amp;page=about </v>
+      </c>
       <c r="F9" s="7" t="str">
         <f>SSP_Regions_32!B9</f>
         <v xml:space="preserve">https://tntcat.iiasa.ac.at/SspDb/dsd?Action=htmlpage&amp;page=about </v>

</xml_diff>